<commit_message>
feat: sort excel by date, project, tags, duration
</commit_message>
<xml_diff>
--- a/generate-excel/src/test/resources/e2e/PiedPiper_2022-01-01_2022-12-31.xlsx
+++ b/generate-excel/src/test/resources/e2e/PiedPiper_2022-01-01_2022-12-31.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tino/IdeaProjects/timesheet-wizard/generate-excel/src/test/resources/e2e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612182DF-672C-3641-8630-8639EF443BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD42C910-B70A-424B-BC26-655B54DE01AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,7 +890,19 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TimeSheet" displayName="TimeSheet" ref="A6:E100" headerRowDxfId="9" dataDxfId="7" totalsRowDxfId="5" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A6:E100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A6:E100" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E62">
+    <sortCondition ref="A7:A100"/>
+    <sortCondition ref="B7:B100"/>
+    <sortCondition ref="C7:C100"/>
+    <sortCondition ref="E7:E100"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" totalsRowLabel="Ergebnis" dataDxfId="4" dataCellStyle="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Project" dataDxfId="3" dataCellStyle="Time"/>
@@ -1171,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1690,10 +1702,10 @@
         <v>11</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E32" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1707,7 +1719,7 @@
         <v>11</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E33" s="17">
         <v>2</v>
@@ -1724,10 +1736,10 @@
         <v>11</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E34" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2149,10 +2161,10 @@
         <v>11</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E59" s="17">
-        <v>1.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2166,10 +2178,10 @@
         <v>11</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E60" s="17">
-        <v>1</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2206,266 +2218,266 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="2"/>
       <c r="E63" s="17"/>
     </row>
-    <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="2"/>
       <c r="E64" s="17"/>
     </row>
-    <row r="65" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="2"/>
       <c r="E65" s="17"/>
     </row>
-    <row r="66" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="2"/>
       <c r="E66" s="17"/>
     </row>
-    <row r="67" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="2"/>
       <c r="E67" s="17"/>
     </row>
-    <row r="68" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="16"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="2"/>
       <c r="E68" s="17"/>
     </row>
-    <row r="69" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="2"/>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="2"/>
       <c r="E70" s="17"/>
     </row>
-    <row r="71" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="2"/>
       <c r="E71" s="17"/>
     </row>
-    <row r="72" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="2"/>
       <c r="E72" s="17"/>
     </row>
-    <row r="73" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="2"/>
       <c r="E73" s="17"/>
     </row>
-    <row r="74" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="2"/>
       <c r="E74" s="17"/>
     </row>
-    <row r="75" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="2"/>
       <c r="E75" s="17"/>
     </row>
-    <row r="76" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="2"/>
       <c r="E76" s="17"/>
     </row>
-    <row r="77" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="2"/>
       <c r="E77" s="17"/>
     </row>
-    <row r="78" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="2"/>
       <c r="E78" s="17"/>
     </row>
-    <row r="79" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="2"/>
       <c r="E79" s="17"/>
     </row>
-    <row r="80" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="2"/>
       <c r="E80" s="17"/>
     </row>
-    <row r="81" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="2"/>
       <c r="E81" s="17"/>
     </row>
-    <row r="82" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="2"/>
       <c r="E82" s="17"/>
     </row>
-    <row r="83" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="2"/>
       <c r="E83" s="17"/>
     </row>
-    <row r="84" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="2"/>
       <c r="E84" s="17"/>
     </row>
-    <row r="85" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="2"/>
       <c r="E85" s="17"/>
     </row>
-    <row r="86" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="2"/>
       <c r="E86" s="17"/>
     </row>
-    <row r="87" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="2"/>
       <c r="E87" s="17"/>
     </row>
-    <row r="88" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="2"/>
       <c r="E88" s="17"/>
     </row>
-    <row r="89" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="2"/>
       <c r="E89" s="17"/>
     </row>
-    <row r="90" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="2"/>
       <c r="E90" s="17"/>
     </row>
-    <row r="91" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="2"/>
       <c r="E91" s="17"/>
     </row>
-    <row r="92" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="2"/>
       <c r="E92" s="17"/>
     </row>
-    <row r="93" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="2"/>
       <c r="E93" s="17"/>
     </row>
-    <row r="94" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="2"/>
       <c r="E94" s="17"/>
     </row>
-    <row r="95" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="2"/>
       <c r="E95" s="17"/>
     </row>
-    <row r="96" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="2"/>
       <c r="E96" s="17"/>
     </row>
-    <row r="97" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="2"/>
       <c r="E97" s="17"/>
     </row>
-    <row r="98" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="16"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="2"/>
       <c r="E98" s="17"/>
     </row>
-    <row r="99" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="16"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="2"/>
       <c r="E99" s="17"/>
     </row>
-    <row r="100" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="18"/>
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
@@ -2479,7 +2491,7 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="D4:E4 F1:XFD1048576 D6:E1048576 A2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>

</xml_diff>